<commit_message>
Add excel referencer app
</commit_message>
<xml_diff>
--- a/server/data/files/excel.xlsx
+++ b/server/data/files/excel.xlsx
@@ -1,18 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18201"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeremy_hewett\Projects\webdav\server\data\files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\webdav\server\data\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FFB6C77-C21E-4ED1-928E-A7189B83BD41}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7500" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sub-est2016_1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0" concurrentCalc="0"/>
   <extLst>
@@ -27,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3337" uniqueCount="663">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3339" uniqueCount="665">
   <si>
     <t>SUMLEV</t>
   </si>
@@ -2017,11 +2019,17 @@
   <si>
     <t>Balance of Winston County</t>
   </si>
+  <si>
+    <t>J</t>
+  </si>
+  <si>
+    <t>JJ</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -3255,12 +3263,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A17:S1122"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -68522,4 +68528,27 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68F75495-2600-448D-99EC-1703D3B91D46}">
+  <dimension ref="B4:J69"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="69" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J69" t="s">
+        <v>664</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>